<commit_message>
made changes to colors and settings in the centers
</commit_message>
<xml_diff>
--- a/data/modified_file.xlsx
+++ b/data/modified_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/AEOE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4581A5E-28AC-F94D-89DF-CFF004804F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9617AB0-DCEC-7A46-88F0-77CC731503F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9841" uniqueCount="3210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9961" uniqueCount="3211">
   <si>
     <t>Organization</t>
   </si>
@@ -179,7 +179,7 @@
     <t>Amigos de Bolsa Chica is a non-profit volunteer organization formed in 1976 by a group of Huntington Beach residents to protect the Bolsa Chica wetlands from development. Located in Huntington Beach in northwest Orange County,  the Bolsa Chica wetlands had once been part of many thousands of acres of coastal wetland that had been filled for urban development in the 20th Century.  Concerned about the statewide loss of wetlands,  the mission of the Amigos de Bolsa Chica is to protect,  preserve and acquire the Bolsa Chica and surrounding open space and to provide education about the importance of wetlands. The Amigos de Bolsa Chica achieved major reductions to the development plans and spearheaded an effort that resulted in the state's acquisition in 1997 of 880 acres of wetlands. The public now owns over 1300 acres of wetland/lowland. A large portion of a major lowland restoration project was completed in 2006. Biodiversity increased almost immediately. The Amigos de Bolsa Chica provides education about this unique ecosystem through private and public wetland tours for schools,  scouts,  other organizations and members of public led by extensively trained Naturalists. Amigos de Bolsa Chica's FLOW Program (Follow and Learn about the Ocean and Wetlands) creates a unique hands-on learning opportunity for students to experience a coastal wetland ecosystem through its most fundamental elements,  water quality and Phytoplankton. By offering bus transportation scholarships to Title 1 schools and underserved,  multicultural students from Huntington Beach and surrounding communities,  the Amigos de Bolsa Chica's education programs expose as diverse an audience as possible to many environmental issues facing the planet through the microcosm of the coastal wetland ecosystem.</t>
   </si>
   <si>
-    <t>18000 Pacific Coast Hwy,  Huntington Beach,  CA 92648</t>
+    <t>18000 Pacific Coast Hwy</t>
   </si>
   <si>
     <t>CA</t>
@@ -242,7 +242,7 @@
     <t>Anza-Borrego Foundation (ABF) is the official nonprofit partner of Anza-Borrego Desert State Park. We provide financial support for Park programs,  acquire land for conservation in and around the Park,  educate the public about the Park’s resources and support research relevant to our region.</t>
   </si>
   <si>
-    <t>587 Palm Canyon Dr #182 San Diego CA 92106 United States</t>
+    <t>587 Palm Canyon Dr #182</t>
   </si>
   <si>
     <t>San Diego</t>
@@ -290,7 +290,7 @@
 ADVANCE - We promote high-quality environmental education among the varied programs across the state and advocate for all young people to experience meaningful learning opportunities outdoors.</t>
   </si>
   <si>
-    <t>1916 Albans Road,  Houston,  TX 77005,  US</t>
+    <t>1916 Albans Road</t>
   </si>
   <si>
     <t>TX</t>
@@ -347,7 +347,7 @@
     <t>Connecting nature,  people,  and science for a more resilient world.</t>
   </si>
   <si>
-    <t>4900 Shoreline Hwy Stinson Beach CA 94970 United States</t>
+    <t xml:space="preserve">4900 Shoreline Hwy </t>
   </si>
   <si>
     <t>Stinson Beach</t>
@@ -390,7 +390,7 @@
 We facilitate a deeper understanding of local ecology and community-learning through place-based education,  inviting children and their families to establish an ongoing relationship with the world we share,  and those we share it with.</t>
   </si>
   <si>
-    <t>1250 Addison St #101 Berkeley CA 94702 United States</t>
+    <t xml:space="preserve">1250 Addison St #101 </t>
   </si>
   <si>
     <t>Berkeley</t>
@@ -438,7 +438,7 @@
     <t>Big Chico Creek Ecological Reserve</t>
   </si>
   <si>
-    <t>3521 14 Mile House Rd Forest Ranch CA 95942 United States</t>
+    <t xml:space="preserve">3521 14 Mile House Rd </t>
   </si>
   <si>
     <t>Forest Ranch</t>
@@ -483,7 +483,7 @@
     <t>Established in 1990 by a coalition of government,  community,  business and environmental leaders,  the Bolsa Chica Conservancy,  a private,  not-for-profit organization,  provides services that inspire and connect all generations through community involvement and leadership in hands-on restoration and education in wetland science,  watersheds,  coastal ecology and environmental sustainability.</t>
   </si>
   <si>
-    <t>3842 Warner Ave Huntington Beach CA 92649-4263 United States</t>
+    <t xml:space="preserve">3842 Warner Ave </t>
   </si>
   <si>
     <t>92649-4263</t>
@@ -601,7 +601,7 @@
     <t>The mission of the California Department of Water Resources (DWR) is to sustainably manage the water resources of California,  in cooperation with other agencies,  to benefit the state's people and protect,  restore,  and enhance the natural and human environments.</t>
   </si>
   <si>
-    <t>715 P Street,  8th Floor Sacramento CA 95817 United States</t>
+    <t>715 P Street</t>
   </si>
   <si>
     <t>Sacramento</t>
@@ -634,7 +634,7 @@
 California is home to the nation’s largest active outdoor industry economy,  contributing $44.5 billion in economic spending annually and 488, 755 direct jobs,  while supporting active lifestyles,  community health and wellness,  and a shared love for California’s majestic outdoors. The California Outdoor Recreation Partnership (CORP) represents the collective interests of member organizations and programs within California,  focused on politics,  policy direction and funding in support of the active outdoor recreation industry. CORP educates legislators about the role that our industry plays in improving economic opportunity,  community health and welcoming a diversity of outdoor enthusiasts across our great state.</t>
   </si>
   <si>
-    <t>6605 San Leandro St Oakland CA 93546 United States</t>
+    <t xml:space="preserve">6605 San Leandro St </t>
   </si>
   <si>
     <t>Oakland</t>
@@ -823,7 +823,7 @@
 Interpretation and Recreation Services Mission: The Interpretive and Recreation Services Department inspires East Bay residents to enjoy and value their Regional Parks through innovative programs and services that are educational,  uplifting and empowering.</t>
   </si>
   <si>
-    <t>2950 Peralta Oaks Ct Oakland CA 94605 United States</t>
+    <t>2950 Peralta Oaks Ct</t>
   </si>
   <si>
     <t>info@ebparks.org</t>
@@ -859,7 +859,7 @@
     <t>ECOLIFE's mission is to protect wildlife,  natural resources,  and the people that depend on them. Founded in 2003,  ECOLIFE Conservation is an international nonprofit organization dedicated to a world where people and nature prosper together. We approach conservation by transforming the way people grow,  access,  and cook food. Our educational programming introduces innovative agriculture and environmental science to classrooms,  while our community-based aquaponic projects support sustainable food systems and increase food security. Since 2014,  ECOLIFE has donated more than 780 ECO-Cycle Aquaponic Kits--along with our K-12 curriculum--to classrooms across the country,  prioritizing Title-1 schools and reaching more than 140, 000 students with hands-on STEM education. ECOLIFE's international efforts focus on building life-saving stoves in rural households in Michoaca?n,  Mexico,  so families can breathe clean air and consume 60% less wood than traditional open-fire cooking.</t>
   </si>
   <si>
-    <t>2810 Pio Pico Dr Carlsbad CA 92008-1521 United States</t>
+    <t>2810 Pio Pico Dr</t>
   </si>
   <si>
     <t>Carlsbad</t>
@@ -994,7 +994,7 @@
     <t>Exploring New Horizons (ENH) engages school groups in 3 to 5-day outdoor education programs that empower students,  build environmental literacy,  and strengthen school communities. Founded as a nonprofit in 1979,  ENH partners with over 100 schools annually,  and in our 43-year history we have served more than 215, 000 students. Each year,  over 7, 000 San Francisco and Monterey Bay Area students participate in programs at our Sempervirens and Pigeon Point sites.</t>
   </si>
   <si>
-    <t>101 Cooper St Santa Cruz CA 95062 United States</t>
+    <t xml:space="preserve">101 Cooper St </t>
   </si>
   <si>
     <t>Santa Cruz</t>
@@ -1061,7 +1061,7 @@
 3) Provide an opportunity for a diverse student population to experience outdoor recreation and develop an appreciation for the forest and its benefits to us all. Extracurricular activities can include a night hike in the woods with a biologist,  zip line,  ride on a narrow gauge railroad,  and evening campfire.</t>
   </si>
   <si>
-    <t>3140 Sierrama Dr Shingle Springs CA 95682 United States</t>
+    <t xml:space="preserve">3140 Sierrama Dr </t>
   </si>
   <si>
     <t>Shingle Springs</t>
@@ -1082,7 +1082,7 @@
     <t>Four Rivers Natural History Association (FRNHA) 501 (c)(3),  as a cooperative association with California State Parks (Four Rivers Sector,  Central Valley District),  supports interpretive and educational programs designed to build human knowledge and connections with natural environments.</t>
   </si>
   <si>
-    <t>Post Office Box 829 Los Banos CA 93635 United States</t>
+    <t xml:space="preserve">Post Office Box 829 </t>
   </si>
   <si>
     <t>Los Banos</t>
@@ -1160,7 +1160,7 @@
     <t>Friends of the Desert Mountains connects people to the land through conservation,  education,  and research. We also support the Santa Rosa and San Jacinto Mountains National Monument.</t>
   </si>
   <si>
-    <t>51500 CA-74 Palm Desert CA 92260 United States</t>
+    <t xml:space="preserve">51500 CA-74 </t>
   </si>
   <si>
     <t>Palm Desert</t>
@@ -1214,7 +1214,7 @@
     <t>Our mission is to protect the beauty of the Fiscalini Ranch Preserve and sustain its diversity of life for everyone to enjoy.</t>
   </si>
   <si>
-    <t>604 Main St Cambria CA 93428-2347 United States</t>
+    <t xml:space="preserve">604 Main St </t>
   </si>
   <si>
     <t>Cambria</t>
@@ -9935,6 +9935,9 @@
   </si>
   <si>
     <t>English, Spanish, French</t>
+  </si>
+  <si>
+    <t>1-19%</t>
   </si>
 </sst>
 </file>
@@ -10304,11 +10307,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="AE105" sqref="AE105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="31" max="31" width="14.83203125" customWidth="1"/>
+    <col min="32" max="32" width="16.83203125" customWidth="1"/>
+    <col min="33" max="33" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -10544,14 +10552,14 @@
       <c r="AG2">
         <v>0</v>
       </c>
-      <c r="AH2" s="2">
-        <v>45310</v>
+      <c r="AH2" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI2">
         <v>0</v>
       </c>
-      <c r="AJ2" s="2">
-        <v>45310</v>
+      <c r="AJ2" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AO2" t="s">
         <v>66</v>
@@ -10657,14 +10665,14 @@
       <c r="AD3" t="s">
         <v>82</v>
       </c>
-      <c r="AE3" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>45310</v>
+      <c r="AE3" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH3" t="s">
         <v>83</v>
@@ -11139,8 +11147,8 @@
       <c r="AE7" t="s">
         <v>101</v>
       </c>
-      <c r="AF7" s="2">
-        <v>45310</v>
+      <c r="AF7" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH7">
         <v>0</v>
@@ -11255,17 +11263,17 @@
       <c r="AD8" t="s">
         <v>161</v>
       </c>
-      <c r="AE8" s="2">
-        <v>45310</v>
+      <c r="AE8" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF8">
         <v>0</v>
       </c>
-      <c r="AG8" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH8" s="2">
-        <v>45310</v>
+      <c r="AG8" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -11942,8 +11950,8 @@
       <c r="AD14" t="s">
         <v>82</v>
       </c>
-      <c r="AE14" s="2">
-        <v>45310</v>
+      <c r="AE14" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF14">
         <v>0</v>
@@ -11951,8 +11959,8 @@
       <c r="AG14" t="s">
         <v>83</v>
       </c>
-      <c r="AH14" s="2">
-        <v>45310</v>
+      <c r="AH14" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI14">
         <v>0</v>
@@ -12061,8 +12069,8 @@
       <c r="AE15" t="s">
         <v>101</v>
       </c>
-      <c r="AF15" s="2">
-        <v>45310</v>
+      <c r="AF15" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG15">
         <v>0</v>
@@ -12201,9 +12209,6 @@
       <c r="AU16" t="s">
         <v>69</v>
       </c>
-      <c r="AW16">
-        <v>2</v>
-      </c>
       <c r="AX16" t="s">
         <v>70</v>
       </c>
@@ -12284,9 +12289,6 @@
       <c r="AR17" t="s">
         <v>67</v>
       </c>
-      <c r="AW17">
-        <v>5</v>
-      </c>
       <c r="AX17" t="s">
         <v>70</v>
       </c>
@@ -12376,8 +12378,8 @@
       <c r="AF18" t="s">
         <v>101</v>
       </c>
-      <c r="AG18" s="2">
-        <v>45310</v>
+      <c r="AG18" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK18" t="s">
         <v>259</v>
@@ -12396,9 +12398,6 @@
       </c>
       <c r="AR18" t="s">
         <v>67</v>
-      </c>
-      <c r="AW18">
-        <v>5</v>
       </c>
       <c r="AX18" t="s">
         <v>70</v>
@@ -12495,9 +12494,6 @@
       <c r="AV19" t="s">
         <v>271</v>
       </c>
-      <c r="AW19">
-        <v>6</v>
-      </c>
       <c r="AX19" t="s">
         <v>70</v>
       </c>
@@ -12590,8 +12586,8 @@
       <c r="AF20">
         <v>0</v>
       </c>
-      <c r="AG20" s="2">
-        <v>45310</v>
+      <c r="AG20" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH20" t="s">
         <v>101</v>
@@ -12622,9 +12618,6 @@
       </c>
       <c r="AU20" t="s">
         <v>69</v>
-      </c>
-      <c r="AW20">
-        <v>8</v>
       </c>
       <c r="AX20" t="s">
         <v>70</v>
@@ -12709,8 +12702,8 @@
       <c r="AD21" t="s">
         <v>284</v>
       </c>
-      <c r="AE21" s="2">
-        <v>45310</v>
+      <c r="AE21" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF21">
         <v>0</v>
@@ -12759,9 +12752,6 @@
       </c>
       <c r="AV21" t="s">
         <v>296</v>
-      </c>
-      <c r="AW21">
-        <v>1</v>
       </c>
       <c r="AX21" t="s">
         <v>70</v>
@@ -12846,11 +12836,11 @@
       <c r="AF22" t="s">
         <v>101</v>
       </c>
-      <c r="AG22" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH22" s="2">
-        <v>45310</v>
+      <c r="AG22" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI22">
         <v>0</v>
@@ -12968,14 +12958,14 @@
       <c r="AE23" t="s">
         <v>101</v>
       </c>
-      <c r="AF23" s="2">
-        <v>45310</v>
+      <c r="AF23" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG23" t="s">
         <v>132</v>
       </c>
-      <c r="AH23" s="2">
-        <v>45310</v>
+      <c r="AH23" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI23">
         <v>0</v>
@@ -13000,9 +12990,6 @@
       </c>
       <c r="AR23" t="s">
         <v>67</v>
-      </c>
-      <c r="AW23">
-        <v>6</v>
       </c>
       <c r="AX23" t="s">
         <v>70</v>
@@ -13093,11 +13080,8 @@
       <c r="AF24">
         <v>0</v>
       </c>
-      <c r="AG24" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AW24">
-        <v>9</v>
+      <c r="AG24" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AX24" t="s">
         <v>70</v>
@@ -13280,9 +13264,6 @@
       <c r="AJ26">
         <v>0</v>
       </c>
-      <c r="AW26">
-        <v>5</v>
-      </c>
       <c r="AX26" t="s">
         <v>70</v>
       </c>
@@ -13488,9 +13469,6 @@
       <c r="AR28" t="s">
         <v>67</v>
       </c>
-      <c r="AW28">
-        <v>9</v>
-      </c>
       <c r="AX28" t="s">
         <v>70</v>
       </c>
@@ -13613,9 +13591,6 @@
       <c r="AV29" t="s">
         <v>367</v>
       </c>
-      <c r="AW29">
-        <v>9</v>
-      </c>
       <c r="AX29" t="s">
         <v>70</v>
       </c>
@@ -13702,11 +13677,11 @@
       <c r="AE30" t="s">
         <v>132</v>
       </c>
-      <c r="AF30" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG30" s="2">
-        <v>45310</v>
+      <c r="AF30" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG30" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH30" t="s">
         <v>101</v>
@@ -13714,8 +13689,8 @@
       <c r="AI30">
         <v>0</v>
       </c>
-      <c r="AJ30" s="2">
-        <v>45310</v>
+      <c r="AJ30" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AO30" t="s">
         <v>66</v>
@@ -13728,9 +13703,6 @@
       </c>
       <c r="AR30" t="s">
         <v>66</v>
-      </c>
-      <c r="AW30">
-        <v>9</v>
       </c>
       <c r="AX30" t="s">
         <v>70</v>
@@ -13824,9 +13796,6 @@
       <c r="AU31" t="s">
         <v>69</v>
       </c>
-      <c r="AW31">
-        <v>9</v>
-      </c>
       <c r="AX31" t="s">
         <v>70</v>
       </c>
@@ -13913,8 +13882,8 @@
       <c r="AF32">
         <v>0</v>
       </c>
-      <c r="AG32" s="2">
-        <v>45310</v>
+      <c r="AG32" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH32">
         <v>0</v>
@@ -13922,8 +13891,8 @@
       <c r="AI32">
         <v>0</v>
       </c>
-      <c r="AJ32" s="2">
-        <v>45310</v>
+      <c r="AJ32" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AO32" t="s">
         <v>69</v>
@@ -13939,9 +13908,6 @@
       </c>
       <c r="AS32" t="s">
         <v>69</v>
-      </c>
-      <c r="AW32">
-        <v>9</v>
       </c>
       <c r="AX32" t="s">
         <v>70</v>
@@ -14035,8 +14001,8 @@
       <c r="AI33" t="s">
         <v>408</v>
       </c>
-      <c r="AJ33" s="2">
-        <v>45310</v>
+      <c r="AJ33" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK33" t="s">
         <v>409</v>
@@ -14064,9 +14030,6 @@
       </c>
       <c r="AU33" t="s">
         <v>69</v>
-      </c>
-      <c r="AW33">
-        <v>9</v>
       </c>
       <c r="AX33" t="s">
         <v>70</v>
@@ -14148,8 +14111,8 @@
       <c r="AF34">
         <v>0</v>
       </c>
-      <c r="AG34" s="2">
-        <v>45310</v>
+      <c r="AG34" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH34">
         <v>0</v>
@@ -14180,9 +14143,6 @@
       </c>
       <c r="AV34" t="s">
         <v>423</v>
-      </c>
-      <c r="AW34">
-        <v>9</v>
       </c>
       <c r="AX34" t="s">
         <v>70</v>
@@ -14297,9 +14257,6 @@
       <c r="AR35" t="s">
         <v>66</v>
       </c>
-      <c r="AW35">
-        <v>9</v>
-      </c>
       <c r="AX35" t="s">
         <v>70</v>
       </c>
@@ -14377,26 +14334,23 @@
       <c r="AD36" t="s">
         <v>148</v>
       </c>
-      <c r="AE36" s="2">
-        <v>45310</v>
+      <c r="AE36" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF36">
         <v>0</v>
       </c>
-      <c r="AG36" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH36" s="2">
-        <v>45310</v>
+      <c r="AG36" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH36" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI36">
         <v>0</v>
       </c>
       <c r="AJ36">
         <v>0</v>
-      </c>
-      <c r="AW36">
-        <v>9</v>
       </c>
       <c r="AX36" t="s">
         <v>70</v>
@@ -14496,11 +14450,11 @@
       <c r="AG37" t="s">
         <v>83</v>
       </c>
-      <c r="AH37" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI37" s="2">
-        <v>45310</v>
+      <c r="AH37" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI37" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ37" t="s">
         <v>83</v>
@@ -14537,9 +14491,6 @@
       </c>
       <c r="AU37" t="s">
         <v>69</v>
-      </c>
-      <c r="AW37">
-        <v>9</v>
       </c>
       <c r="AX37" t="s">
         <v>70</v>
@@ -14749,8 +14700,8 @@
       <c r="AI39" t="s">
         <v>83</v>
       </c>
-      <c r="AJ39" s="2">
-        <v>45310</v>
+      <c r="AJ39" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK39" t="s">
         <v>474</v>
@@ -14769,9 +14720,6 @@
       </c>
       <c r="AR39" t="s">
         <v>67</v>
-      </c>
-      <c r="AW39">
-        <v>9</v>
       </c>
       <c r="AX39" t="s">
         <v>70</v>
@@ -14859,14 +14807,11 @@
       <c r="AH40">
         <v>0</v>
       </c>
-      <c r="AI40" s="2">
-        <v>45310</v>
+      <c r="AI40" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ40" t="s">
         <v>101</v>
-      </c>
-      <c r="AW40">
-        <v>9</v>
       </c>
       <c r="AX40" t="s">
         <v>70</v>
@@ -14960,11 +14905,11 @@
       <c r="AG41" t="s">
         <v>83</v>
       </c>
-      <c r="AH41" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI41" s="2">
-        <v>45310</v>
+      <c r="AH41" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI41" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ41" t="s">
         <v>83</v>
@@ -14998,9 +14943,6 @@
       </c>
       <c r="AU41" t="s">
         <v>69</v>
-      </c>
-      <c r="AW41">
-        <v>9</v>
       </c>
       <c r="AX41" t="s">
         <v>70</v>
@@ -15115,9 +15057,6 @@
       <c r="AV42" t="s">
         <v>506</v>
       </c>
-      <c r="AW42">
-        <v>9</v>
-      </c>
       <c r="AX42" t="s">
         <v>70</v>
       </c>
@@ -15204,11 +15143,11 @@
       <c r="AD43" t="s">
         <v>161</v>
       </c>
-      <c r="AE43" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF43" s="2">
-        <v>45310</v>
+      <c r="AE43" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF43" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK43" t="s">
         <v>518</v>
@@ -15230,9 +15169,6 @@
       </c>
       <c r="AS43" t="s">
         <v>69</v>
-      </c>
-      <c r="AW43">
-        <v>9</v>
       </c>
       <c r="AX43" t="s">
         <v>70</v>
@@ -15314,8 +15250,8 @@
       <c r="AD44" t="s">
         <v>130</v>
       </c>
-      <c r="AE44" s="2">
-        <v>45310</v>
+      <c r="AE44" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH44">
         <v>0</v>
@@ -15352,9 +15288,6 @@
       </c>
       <c r="AU44" t="s">
         <v>69</v>
-      </c>
-      <c r="AW44">
-        <v>8</v>
       </c>
       <c r="AX44" t="s">
         <v>70</v>
@@ -15436,14 +15369,14 @@
       <c r="AD45" t="s">
         <v>284</v>
       </c>
-      <c r="AE45" s="2">
-        <v>45310</v>
+      <c r="AE45" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF45">
         <v>0</v>
       </c>
-      <c r="AG45" s="2">
-        <v>45310</v>
+      <c r="AG45" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AM45" t="s">
         <v>84</v>
@@ -15459,9 +15392,6 @@
       </c>
       <c r="AR45" t="s">
         <v>66</v>
-      </c>
-      <c r="AW45">
-        <v>12</v>
       </c>
       <c r="AX45" t="s">
         <v>70</v>
@@ -15525,9 +15455,6 @@
       <c r="W46" t="s">
         <v>117</v>
       </c>
-      <c r="AW46">
-        <v>8</v>
-      </c>
       <c r="AX46" t="s">
         <v>70</v>
       </c>
@@ -15611,23 +15538,20 @@
       <c r="AD47" t="s">
         <v>148</v>
       </c>
-      <c r="AE47" s="2">
-        <v>45310</v>
+      <c r="AE47" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF47">
         <v>0</v>
       </c>
-      <c r="AG47" s="2">
-        <v>45310</v>
+      <c r="AG47" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI47">
         <v>0</v>
       </c>
-      <c r="AJ47" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AW47">
-        <v>13</v>
+      <c r="AJ47" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AX47" t="s">
         <v>70</v>
@@ -15721,9 +15645,6 @@
       <c r="AV48" t="s">
         <v>561</v>
       </c>
-      <c r="AW48">
-        <v>8</v>
-      </c>
       <c r="AX48" t="s">
         <v>70</v>
       </c>
@@ -15804,23 +15725,23 @@
       <c r="AD49" t="s">
         <v>148</v>
       </c>
-      <c r="AE49" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF49" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG49" s="2">
-        <v>45310</v>
+      <c r="AE49" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF49" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG49" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH49" t="s">
         <v>101</v>
       </c>
-      <c r="AI49" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AJ49" s="2">
-        <v>45310</v>
+      <c r="AI49" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AJ49" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK49" t="s">
         <v>571</v>
@@ -15932,8 +15853,8 @@
       <c r="AE50" t="s">
         <v>132</v>
       </c>
-      <c r="AF50" s="2">
-        <v>45310</v>
+      <c r="AF50" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG50" t="s">
         <v>83</v>
@@ -15979,9 +15900,6 @@
       </c>
       <c r="AU50" t="s">
         <v>69</v>
-      </c>
-      <c r="AW50">
-        <v>8</v>
       </c>
       <c r="AX50" t="s">
         <v>70</v>
@@ -16075,17 +15993,14 @@
       <c r="AF51">
         <v>0</v>
       </c>
-      <c r="AG51" s="2">
-        <v>45310</v>
+      <c r="AG51" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH51" t="s">
         <v>101</v>
       </c>
       <c r="AI51" t="s">
         <v>101</v>
-      </c>
-      <c r="AW51">
-        <v>8</v>
       </c>
       <c r="AX51" t="s">
         <v>70</v>
@@ -16155,9 +16070,6 @@
       <c r="AJ52">
         <v>0</v>
       </c>
-      <c r="AW52">
-        <v>11</v>
-      </c>
       <c r="AX52" t="s">
         <v>70</v>
       </c>
@@ -16244,17 +16156,14 @@
       <c r="AG53">
         <v>0</v>
       </c>
-      <c r="AH53" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI53" s="2">
-        <v>45310</v>
+      <c r="AH53" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI53" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ53">
         <v>0</v>
-      </c>
-      <c r="AW53">
-        <v>4</v>
       </c>
       <c r="AX53" t="s">
         <v>70</v>
@@ -16315,9 +16224,6 @@
       <c r="W54" t="s">
         <v>117</v>
       </c>
-      <c r="AW54">
-        <v>9</v>
-      </c>
       <c r="AX54" t="s">
         <v>70</v>
       </c>
@@ -16449,9 +16355,6 @@
       <c r="AV55" t="s">
         <v>634</v>
       </c>
-      <c r="AW55">
-        <v>4</v>
-      </c>
       <c r="AX55" t="s">
         <v>70</v>
       </c>
@@ -16538,11 +16441,11 @@
       <c r="AD56" t="s">
         <v>148</v>
       </c>
-      <c r="AE56" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH56" s="2">
-        <v>45310</v>
+      <c r="AE56" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH56" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AO56" t="s">
         <v>67</v>
@@ -16555,9 +16458,6 @@
       </c>
       <c r="AR56" t="s">
         <v>66</v>
-      </c>
-      <c r="AW56">
-        <v>4</v>
       </c>
       <c r="AX56" t="s">
         <v>70</v>
@@ -16669,9 +16569,6 @@
       <c r="AS57" t="s">
         <v>67</v>
       </c>
-      <c r="AW57">
-        <v>8</v>
-      </c>
       <c r="AX57" t="s">
         <v>70</v>
       </c>
@@ -16898,9 +16795,6 @@
       <c r="AU59" t="s">
         <v>69</v>
       </c>
-      <c r="AW59">
-        <v>5</v>
-      </c>
       <c r="AX59" t="s">
         <v>70</v>
       </c>
@@ -16999,9 +16893,6 @@
       <c r="AJ60">
         <v>0</v>
       </c>
-      <c r="AW60">
-        <v>4</v>
-      </c>
       <c r="AX60" t="s">
         <v>70</v>
       </c>
@@ -17246,9 +17137,6 @@
       <c r="AU62" t="s">
         <v>69</v>
       </c>
-      <c r="AW62">
-        <v>9</v>
-      </c>
       <c r="AX62" t="s">
         <v>70</v>
       </c>
@@ -17329,23 +17217,20 @@
       <c r="AE63">
         <v>0</v>
       </c>
-      <c r="AF63" s="2">
-        <v>45310</v>
+      <c r="AF63" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG63" t="s">
         <v>132</v>
       </c>
-      <c r="AH63" s="2">
-        <v>45310</v>
+      <c r="AH63" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI63">
         <v>0</v>
       </c>
       <c r="AJ63">
         <v>0</v>
-      </c>
-      <c r="AW63">
-        <v>9</v>
       </c>
       <c r="AX63" t="s">
         <v>70</v>
@@ -17478,9 +17363,6 @@
       <c r="AU64" t="s">
         <v>69</v>
       </c>
-      <c r="AW64">
-        <v>9</v>
-      </c>
       <c r="AX64" t="s">
         <v>70</v>
       </c>
@@ -17567,26 +17449,23 @@
       <c r="AD65" t="s">
         <v>148</v>
       </c>
-      <c r="AE65" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF65" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG65" s="2">
-        <v>45310</v>
+      <c r="AE65" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF65" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG65" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH65" t="s">
         <v>83</v>
       </c>
-      <c r="AI65" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AJ65" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AW65">
-        <v>2</v>
+      <c r="AI65" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AJ65" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AX65" t="s">
         <v>70</v>
@@ -17719,9 +17598,6 @@
       <c r="AU66" t="s">
         <v>69</v>
       </c>
-      <c r="AW66">
-        <v>8</v>
-      </c>
       <c r="AX66" t="s">
         <v>70</v>
       </c>
@@ -17832,9 +17708,6 @@
       <c r="AU67" t="s">
         <v>69</v>
       </c>
-      <c r="AW67">
-        <v>2</v>
-      </c>
       <c r="AX67" t="s">
         <v>70</v>
       </c>
@@ -17966,9 +17839,6 @@
       <c r="AU68" t="s">
         <v>69</v>
       </c>
-      <c r="AW68">
-        <v>8</v>
-      </c>
       <c r="AX68" t="s">
         <v>70</v>
       </c>
@@ -18073,9 +17943,6 @@
       <c r="AR69" t="s">
         <v>67</v>
       </c>
-      <c r="AW69">
-        <v>9</v>
-      </c>
       <c r="AX69" t="s">
         <v>70</v>
       </c>
@@ -18165,11 +18032,11 @@
       <c r="AG70" t="s">
         <v>101</v>
       </c>
-      <c r="AH70" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI70" s="2">
-        <v>45310</v>
+      <c r="AH70" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI70" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ70" t="s">
         <v>83</v>
@@ -18197,9 +18064,6 @@
       </c>
       <c r="AV70" t="s">
         <v>796</v>
-      </c>
-      <c r="AW70">
-        <v>5</v>
       </c>
       <c r="AX70" t="s">
         <v>70</v>
@@ -18275,23 +18139,23 @@
       <c r="AD71" t="s">
         <v>148</v>
       </c>
-      <c r="AE71" s="2">
-        <v>45310</v>
+      <c r="AE71" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF71">
         <v>0</v>
       </c>
-      <c r="AG71" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH71" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI71" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AJ71" s="2">
-        <v>45310</v>
+      <c r="AG71" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH71" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI71" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AJ71" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK71" t="s">
         <v>505</v>
@@ -18394,11 +18258,11 @@
       <c r="AD72" t="s">
         <v>161</v>
       </c>
-      <c r="AE72" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF72" s="2">
-        <v>45310</v>
+      <c r="AE72" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF72" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH72">
         <v>0</v>
@@ -18733,8 +18597,8 @@
       <c r="AF75">
         <v>0</v>
       </c>
-      <c r="AG75" s="2">
-        <v>45310</v>
+      <c r="AG75" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH75">
         <v>0</v>
@@ -18843,23 +18707,23 @@
       <c r="AD76" t="s">
         <v>284</v>
       </c>
-      <c r="AE76" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF76" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG76" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH76" s="2">
-        <v>45310</v>
+      <c r="AE76" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF76" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG76" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH76" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI76">
         <v>0</v>
       </c>
-      <c r="AJ76" s="2">
-        <v>45310</v>
+      <c r="AJ76" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AM76" t="s">
         <v>84</v>
@@ -18959,8 +18823,8 @@
       <c r="AD77" t="s">
         <v>161</v>
       </c>
-      <c r="AE77" s="2">
-        <v>45310</v>
+      <c r="AE77" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF77">
         <v>0</v>
@@ -18971,8 +18835,8 @@
       <c r="AH77">
         <v>0</v>
       </c>
-      <c r="AI77" s="2">
-        <v>45310</v>
+      <c r="AI77" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ77">
         <v>0</v>
@@ -19069,8 +18933,8 @@
       <c r="AE78" t="s">
         <v>101</v>
       </c>
-      <c r="AF78" s="2">
-        <v>45310</v>
+      <c r="AF78" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG78" t="s">
         <v>101</v>
@@ -19307,8 +19171,8 @@
       <c r="AG80">
         <v>0</v>
       </c>
-      <c r="AH80" s="2">
-        <v>45310</v>
+      <c r="AH80" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI80">
         <v>0</v>
@@ -19518,8 +19382,8 @@
       <c r="AF82">
         <v>0</v>
       </c>
-      <c r="AG82" s="2">
-        <v>45310</v>
+      <c r="AG82" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH82">
         <v>0</v>
@@ -19649,8 +19513,8 @@
       <c r="AH83" t="s">
         <v>101</v>
       </c>
-      <c r="AI83" s="2">
-        <v>45310</v>
+      <c r="AI83" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ83" t="s">
         <v>83</v>
@@ -19768,8 +19632,8 @@
       <c r="AF84" t="s">
         <v>131</v>
       </c>
-      <c r="AG84" s="2">
-        <v>45310</v>
+      <c r="AG84" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH84" t="s">
         <v>101</v>
@@ -19884,11 +19748,11 @@
       <c r="AE85" t="s">
         <v>132</v>
       </c>
-      <c r="AF85" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG85" s="2">
-        <v>45310</v>
+      <c r="AF85" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG85" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH85" t="s">
         <v>83</v>
@@ -20012,8 +19876,8 @@
       <c r="AD86" t="s">
         <v>284</v>
       </c>
-      <c r="AE86" s="2">
-        <v>45310</v>
+      <c r="AE86" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF86">
         <v>0</v>
@@ -20140,8 +20004,8 @@
       <c r="AF87">
         <v>0</v>
       </c>
-      <c r="AG87" s="2">
-        <v>45310</v>
+      <c r="AG87" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH87">
         <v>0</v>
@@ -20149,8 +20013,8 @@
       <c r="AI87">
         <v>0</v>
       </c>
-      <c r="AJ87" s="2">
-        <v>45310</v>
+      <c r="AJ87" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AX87" t="s">
         <v>70</v>
@@ -20351,8 +20215,8 @@
       <c r="AF89">
         <v>0</v>
       </c>
-      <c r="AG89" s="2">
-        <v>45310</v>
+      <c r="AG89" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH89">
         <v>0</v>
@@ -20360,8 +20224,8 @@
       <c r="AI89">
         <v>0</v>
       </c>
-      <c r="AJ89" s="2">
-        <v>45310</v>
+      <c r="AJ89" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AO89" t="s">
         <v>66</v>
@@ -20467,8 +20331,8 @@
       <c r="AF90">
         <v>0</v>
       </c>
-      <c r="AG90" s="2">
-        <v>45310</v>
+      <c r="AG90" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH90">
         <v>0</v>
@@ -20803,20 +20667,20 @@
       <c r="AD93" t="s">
         <v>130</v>
       </c>
-      <c r="AE93" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF93" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AG93" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH93" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI93" s="2">
-        <v>45310</v>
+      <c r="AE93" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF93" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AG93" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH93" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI93" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AJ93" t="s">
         <v>83</v>
@@ -20925,8 +20789,8 @@
       <c r="AE94" t="s">
         <v>101</v>
       </c>
-      <c r="AF94" s="2">
-        <v>45310</v>
+      <c r="AF94" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG94" t="s">
         <v>131</v>
@@ -21032,23 +20896,23 @@
       <c r="AD95" t="s">
         <v>148</v>
       </c>
-      <c r="AE95" s="2">
-        <v>45310</v>
+      <c r="AE95" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF95" t="s">
         <v>131</v>
       </c>
-      <c r="AG95" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH95" s="2">
-        <v>45310</v>
+      <c r="AG95" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH95" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI95">
         <v>0</v>
       </c>
-      <c r="AJ95" s="2">
-        <v>45310</v>
+      <c r="AJ95" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK95" t="s">
         <v>1035</v>
@@ -21163,8 +21027,8 @@
       <c r="AI96" t="s">
         <v>101</v>
       </c>
-      <c r="AJ96" s="2">
-        <v>45310</v>
+      <c r="AJ96" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK96" t="s">
         <v>474</v>
@@ -21279,8 +21143,8 @@
       <c r="AD97" t="s">
         <v>148</v>
       </c>
-      <c r="AE97" s="2">
-        <v>45310</v>
+      <c r="AE97" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF97">
         <v>0</v>
@@ -21288,14 +21152,14 @@
       <c r="AG97">
         <v>0</v>
       </c>
-      <c r="AH97" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AI97" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AJ97" s="2">
-        <v>45310</v>
+      <c r="AH97" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AI97" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AJ97" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AO97" t="s">
         <v>66</v>
@@ -21404,8 +21268,8 @@
       <c r="AF98">
         <v>0</v>
       </c>
-      <c r="AG98" s="2">
-        <v>45310</v>
+      <c r="AG98" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH98" t="s">
         <v>83</v>
@@ -21514,8 +21378,8 @@
       <c r="AD99" t="s">
         <v>284</v>
       </c>
-      <c r="AE99" s="2">
-        <v>45310</v>
+      <c r="AE99" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF99">
         <v>0</v>
@@ -21523,8 +21387,8 @@
       <c r="AH99" t="s">
         <v>101</v>
       </c>
-      <c r="AI99" s="2">
-        <v>45310</v>
+      <c r="AI99" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AK99" t="s">
         <v>505</v>
@@ -21630,11 +21494,11 @@
       <c r="AD100" t="s">
         <v>284</v>
       </c>
-      <c r="AE100" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AF100" s="2">
-        <v>45310</v>
+      <c r="AE100" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AF100" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AG100">
         <v>0</v>
@@ -21642,8 +21506,8 @@
       <c r="AH100" t="s">
         <v>101</v>
       </c>
-      <c r="AI100" s="2">
-        <v>45310</v>
+      <c r="AI100" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AX100" t="s">
         <v>70</v>
@@ -21871,14 +21735,14 @@
       <c r="AG102" t="s">
         <v>408</v>
       </c>
-      <c r="AH102" s="2">
-        <v>45310</v>
+      <c r="AH102" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI102">
         <v>0</v>
       </c>
-      <c r="AJ102" s="2">
-        <v>45310</v>
+      <c r="AJ102" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AX102" t="s">
         <v>70</v>
@@ -21963,11 +21827,11 @@
       <c r="AF103" t="s">
         <v>101</v>
       </c>
-      <c r="AG103" s="2">
-        <v>45310</v>
-      </c>
-      <c r="AH103" s="2">
-        <v>45310</v>
+      <c r="AG103" s="2" t="s">
+        <v>3210</v>
+      </c>
+      <c r="AH103" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AI103">
         <v>0</v>
@@ -22055,8 +21919,8 @@
       <c r="AF104">
         <v>0</v>
       </c>
-      <c r="AG104" s="2">
-        <v>45310</v>
+      <c r="AG104" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH104">
         <v>0</v>
@@ -22153,14 +22017,14 @@
       <c r="AD105" t="s">
         <v>100</v>
       </c>
-      <c r="AE105" s="2">
-        <v>45310</v>
+      <c r="AE105" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AF105">
         <v>0</v>
       </c>
-      <c r="AG105" s="2">
-        <v>45310</v>
+      <c r="AG105" s="2" t="s">
+        <v>3210</v>
       </c>
       <c r="AH105">
         <v>0</v>

</xml_diff>